<commit_message>
Một số thay đổi
</commit_message>
<xml_diff>
--- a/02_data_description.xlsx
+++ b/02_data_description.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bffdd9d9aa3c737/Documents/Collage boy/DSTC/Vòng 2/DSTC_bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC884702-B35C-45DA-BB4B-29560E2542C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{17C4AAEF-C4BC-4D7A-8534-EF82AD942595}"/>
+    <workbookView minimized="1" xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" xr2:uid="{17C4AAEF-C4BC-4D7A-8534-EF82AD942595}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,11 +173,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -185,7 +185,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -252,9 +252,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -292,7 +292,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -398,7 +398,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -540,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -551,16 +551,16 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="45.453125" customWidth="1"/>
-    <col min="2" max="2" width="108.36328125" customWidth="1"/>
+    <col min="1" max="1" width="45.5" customWidth="1"/>
+    <col min="2" max="2" width="108.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -568,7 +568,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -576,7 +576,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="31.5" customHeight="1">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -584,7 +584,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -592,7 +592,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
@@ -600,7 +600,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -608,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -616,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -624,7 +624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -632,7 +632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -640,7 +640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -648,7 +648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -656,7 +656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -664,7 +664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -672,7 +672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>26</v>
       </c>
@@ -680,7 +680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -688,7 +688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
@@ -696,7 +696,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -704,7 +704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>34</v>
       </c>
@@ -712,7 +712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>36</v>
       </c>
@@ -720,7 +720,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
         <v>38</v>
       </c>
@@ -728,7 +728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
         <v>40</v>
       </c>

</xml_diff>

<commit_message>
use building a scorecard model.ipynb
</commit_message>
<xml_diff>
--- a/02_data_description.xlsx
+++ b/02_data_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2bffdd9d9aa3c737/Documents/Collage boy/DSTC/Vòng 2/DSTC_bank/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC884702-B35C-45DA-BB4B-29560E2542C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{DC884702-B35C-45DA-BB4B-29560E2542C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDC8FA8D-75A1-4967-8FCC-6C87F5122E5B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2580" yWindow="2580" windowWidth="17280" windowHeight="8880" xr2:uid="{17C4AAEF-C4BC-4D7A-8534-EF82AD942595}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{17C4AAEF-C4BC-4D7A-8534-EF82AD942595}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -550,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ABDAD71-D6BD-4BE1-B7B5-67127E67C67C}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="72" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>